<commit_message>
adding activity log in application
</commit_message>
<xml_diff>
--- a/backend-status-burnin/Burnin Shift Activities.xlsx
+++ b/backend-status-burnin/Burnin Shift Activities.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Shift 2 - 2025-02-17" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Shift 2 - 2025-02-18" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Engineer</t>
   </si>
   <si>
-    <t>2025-02-17</t>
+    <t>2025-02-18</t>
   </si>
   <si>
     <t>RESPALDO DE BASE DE DATOS</t>
@@ -40,16 +40,25 @@
     <t>Renato Hacel Cal y Mayor Rodríguez, Administrador</t>
   </si>
   <si>
+    <t>GRR EN LA SECCION 6</t>
+  </si>
+  <si>
+    <t>Esta si tiene descripcion</t>
+  </si>
+  <si>
+    <t>REINICIO DE BIOS 3</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
     <t>EJECUTAR GRR</t>
   </si>
   <si>
     <t>GRR 2H-23 2H-38</t>
-  </si>
-  <si>
-    <t>REINICIO DE BIOS 3</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -448,7 +457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
@@ -523,7 +532,24 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>